<commit_message>
Missing cases and 4 Soviet countries fixed.
</commit_message>
<xml_diff>
--- a/results/Tbl1.xlsx
+++ b/results/Tbl1.xlsx
@@ -111,9 +111,6 @@
     <t>0.002*</t>
   </si>
   <si>
-    <t>0.006*</t>
-  </si>
-  <si>
     <t>0.004*</t>
   </si>
   <si>
@@ -148,6 +145,9 @@
   </si>
   <si>
     <t>AIC</t>
+  </si>
+  <si>
+    <t>0.007*</t>
   </si>
 </sst>
 </file>
@@ -655,9 +655,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -675,6 +672,9 @@
     </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="42">
@@ -1000,7 +1000,7 @@
   <dimension ref="A3:G23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:G23"/>
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -1010,409 +1010,409 @@
   </cols>
   <sheetData>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="C3" s="9"/>
+      <c r="D3" s="9"/>
+      <c r="E3" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="C3" s="2"/>
-      <c r="D3" s="2"/>
-      <c r="E3" s="2" t="s">
+      <c r="F3" s="9"/>
+      <c r="G3" s="9"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="B4" s="3"/>
+      <c r="C4" s="3"/>
+      <c r="D4" s="3"/>
+      <c r="E4" s="3"/>
+      <c r="F4" s="3"/>
+      <c r="G4" s="3"/>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="G9" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="B10" s="2"/>
+      <c r="C10" s="2"/>
+      <c r="D10" s="2"/>
+      <c r="E10" s="2"/>
+      <c r="F10" s="2"/>
+      <c r="G10" s="2"/>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="B11" s="8"/>
+      <c r="C11" s="8">
+        <v>1.325</v>
+      </c>
+      <c r="D11" s="8">
+        <v>1.401</v>
+      </c>
+      <c r="E11" s="8"/>
+      <c r="F11" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="G11" s="8" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D12" s="2">
+        <v>11.584</v>
+      </c>
+      <c r="E12" s="2">
+        <v>14.135999999999999</v>
+      </c>
+      <c r="F12" s="2">
+        <v>24.440999999999999</v>
+      </c>
+      <c r="G12" s="2">
+        <v>2.6920000000000002</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B13" s="2">
+        <v>1.2290000000000001</v>
+      </c>
+      <c r="C13" s="2">
+        <v>1.121</v>
+      </c>
+      <c r="D13" s="2">
+        <v>0.34899999999999998</v>
+      </c>
+      <c r="E13" s="2">
+        <v>0.152</v>
+      </c>
+      <c r="F13" s="2">
+        <v>8.5000000000000006E-2</v>
+      </c>
+      <c r="G13" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B14" s="2">
+        <v>1.026</v>
+      </c>
+      <c r="C14" s="2">
+        <v>1.0069999999999999</v>
+      </c>
+      <c r="D14" s="2">
+        <v>0.83899999999999997</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="G14" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B15" s="2"/>
+      <c r="C15" s="2"/>
+      <c r="D15" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E15" s="2"/>
+      <c r="F15" s="2"/>
+      <c r="G15" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="F3" s="2"/>
-      <c r="G3" s="2"/>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="5" t="s">
+      <c r="B16" s="2">
+        <v>0.98499999999999999</v>
+      </c>
+      <c r="C16" s="2">
+        <v>0.98199999999999998</v>
+      </c>
+      <c r="D16" s="2">
+        <v>1.002</v>
+      </c>
+      <c r="E16" s="2">
+        <v>0.90600000000000003</v>
+      </c>
+      <c r="F16" s="2">
+        <v>0.91500000000000004</v>
+      </c>
+      <c r="G16" s="2">
+        <v>0.89500000000000002</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="F17" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="G17" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="B4" s="4"/>
-      <c r="C4" s="4"/>
-      <c r="D4" s="4"/>
-      <c r="E4" s="4"/>
-      <c r="F4" s="4"/>
-      <c r="G4" s="4"/>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="F5" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="G5" s="3" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="F6" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="G6" s="3" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="E7" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="F7" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="G7" s="3" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="B8" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="D8" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="E8" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="F8" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="G8" s="3" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="B9" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="C9" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="D9" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="E9" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="F9" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="G9" s="3" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="5" t="s">
+      <c r="B18" s="2"/>
+      <c r="C18" s="2"/>
+      <c r="D18" s="2"/>
+      <c r="E18" s="2"/>
+      <c r="F18" s="2"/>
+      <c r="G18" s="2"/>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B19" s="2">
+        <v>164</v>
+      </c>
+      <c r="C19" s="2">
+        <v>164</v>
+      </c>
+      <c r="D19" s="2">
+        <v>164</v>
+      </c>
+      <c r="E19" s="2">
+        <v>164</v>
+      </c>
+      <c r="F19" s="2">
+        <v>164</v>
+      </c>
+      <c r="G19" s="2">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B20" s="6">
+        <v>7870</v>
+      </c>
+      <c r="C20" s="6">
+        <v>7870</v>
+      </c>
+      <c r="D20" s="6">
+        <v>7870</v>
+      </c>
+      <c r="E20" s="6">
+        <v>12269</v>
+      </c>
+      <c r="F20" s="6">
+        <v>12269</v>
+      </c>
+      <c r="G20" s="6">
+        <v>12269</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B21" s="2">
+        <v>-657.15</v>
+      </c>
+      <c r="C21" s="2">
+        <v>-656.87</v>
+      </c>
+      <c r="D21" s="2">
+        <v>-651.42200000000003</v>
+      </c>
+      <c r="E21" s="2">
+        <v>-651.74699999999996</v>
+      </c>
+      <c r="F21" s="2">
+        <v>-647.375</v>
+      </c>
+      <c r="G21" s="2">
+        <v>-642.31399999999996</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="B10" s="3"/>
-      <c r="C10" s="3"/>
-      <c r="D10" s="3"/>
-      <c r="E10" s="3"/>
-      <c r="F10" s="3"/>
-      <c r="G10" s="3"/>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="B11" s="9"/>
-      <c r="C11" s="9">
-        <v>1.325</v>
-      </c>
-      <c r="D11" s="9">
-        <v>1.401</v>
-      </c>
-      <c r="E11" s="9"/>
-      <c r="F11" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="G11" s="9" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="B12" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="C12" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="D12" s="3">
-        <v>11.584</v>
-      </c>
-      <c r="E12" s="3">
-        <v>14.135999999999999</v>
-      </c>
-      <c r="F12" s="3">
-        <v>24.440999999999999</v>
-      </c>
-      <c r="G12" s="3">
-        <v>2.6920000000000002</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="B13" s="3">
-        <v>1.2290000000000001</v>
-      </c>
-      <c r="C13" s="3">
-        <v>1.121</v>
-      </c>
-      <c r="D13" s="3">
-        <v>0.34899999999999998</v>
-      </c>
-      <c r="E13" s="3">
-        <v>0.152</v>
-      </c>
-      <c r="F13" s="3">
-        <v>8.5000000000000006E-2</v>
-      </c>
-      <c r="G13" s="3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="B14" s="3">
-        <v>1.026</v>
-      </c>
-      <c r="C14" s="3">
-        <v>1.0069999999999999</v>
-      </c>
-      <c r="D14" s="3">
-        <v>0.83899999999999997</v>
-      </c>
-      <c r="E14" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="F14" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="G14" s="3" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="B15" s="3"/>
-      <c r="C15" s="3"/>
-      <c r="D15" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="E15" s="3"/>
-      <c r="F15" s="3"/>
-      <c r="G15" s="3" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="B16" s="3">
-        <v>0.98499999999999999</v>
-      </c>
-      <c r="C16" s="3">
-        <v>0.98199999999999998</v>
-      </c>
-      <c r="D16" s="3">
-        <v>1.002</v>
-      </c>
-      <c r="E16" s="3">
-        <v>0.90600000000000003</v>
-      </c>
-      <c r="F16" s="3">
-        <v>0.91500000000000004</v>
-      </c>
-      <c r="G16" s="3">
-        <v>0.89500000000000002</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="B17" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="C17" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="D17" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="E17" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="F17" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="G17" s="3" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="B18" s="3"/>
-      <c r="C18" s="3"/>
-      <c r="D18" s="3"/>
-      <c r="E18" s="3"/>
-      <c r="F18" s="3"/>
-      <c r="G18" s="3"/>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="B19" s="3">
-        <v>164</v>
-      </c>
-      <c r="C19" s="3">
-        <v>164</v>
-      </c>
-      <c r="D19" s="3">
-        <v>164</v>
-      </c>
-      <c r="E19" s="3">
-        <v>164</v>
-      </c>
-      <c r="F19" s="3">
-        <v>164</v>
-      </c>
-      <c r="G19" s="3">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="B20" s="7">
-        <v>7870</v>
-      </c>
-      <c r="C20" s="7">
-        <v>7870</v>
-      </c>
-      <c r="D20" s="7">
-        <v>7870</v>
-      </c>
-      <c r="E20" s="7">
-        <v>12269</v>
-      </c>
-      <c r="F20" s="7">
-        <v>12269</v>
-      </c>
-      <c r="G20" s="7">
-        <v>12269</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A21" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="B21" s="3">
-        <v>-657.15</v>
-      </c>
-      <c r="C21" s="3">
-        <v>-656.87</v>
-      </c>
-      <c r="D21" s="3">
-        <v>-651.42200000000003</v>
-      </c>
-      <c r="E21" s="3">
-        <v>-651.74699999999996</v>
-      </c>
-      <c r="F21" s="3">
-        <v>-647.375</v>
-      </c>
-      <c r="G21" s="3">
-        <v>-642.31399999999996</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A22" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="B22" s="3">
+      <c r="B22" s="2">
         <v>1334.299</v>
       </c>
-      <c r="C22" s="3">
+      <c r="C22" s="2">
         <v>1335.739</v>
       </c>
-      <c r="D22" s="3">
+      <c r="D22" s="2">
         <v>1326.8430000000001</v>
       </c>
-      <c r="E22" s="3">
+      <c r="E22" s="2">
         <v>1323.4939999999999</v>
       </c>
-      <c r="F22" s="3">
+      <c r="F22" s="2">
         <v>1316.751</v>
       </c>
-      <c r="G22" s="3">
+      <c r="G22" s="2">
         <v>1308.6279999999999</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
New Fig1 treatment plot
</commit_message>
<xml_diff>
--- a/results/Tbl1.xlsx
+++ b/results/Tbl1.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="45">
   <si>
     <t>(1880-1902)</t>
   </si>
@@ -42,12 +42,6 @@
     <t>Network Exposure: Culture (t-1)</t>
   </si>
   <si>
-    <t>Network Exposure: Colonial</t>
-  </si>
-  <si>
-    <t>0.039+</t>
-  </si>
-  <si>
     <t>Network Exposure: Trade (t-1)</t>
   </si>
   <si>
@@ -63,48 +57,12 @@
     <t>Log Likelihood</t>
   </si>
   <si>
-    <t>30.936*</t>
-  </si>
-  <si>
     <t>Countries</t>
   </si>
   <si>
-    <t>1.260*</t>
-  </si>
-  <si>
     <t>1.160*</t>
   </si>
   <si>
-    <t>1.140*</t>
-  </si>
-  <si>
-    <t>1.144*</t>
-  </si>
-  <si>
-    <t>37.793*</t>
-  </si>
-  <si>
-    <t>1.283*</t>
-  </si>
-  <si>
-    <t>1.290*</t>
-  </si>
-  <si>
-    <t>5.304*</t>
-  </si>
-  <si>
-    <t>7.085*</t>
-  </si>
-  <si>
-    <t>7.648*</t>
-  </si>
-  <si>
-    <t>72.377*</t>
-  </si>
-  <si>
-    <t>71.811*</t>
-  </si>
-  <si>
     <t>0.001*</t>
   </si>
   <si>
@@ -117,12 +75,6 @@
     <t>0.003*</t>
   </si>
   <si>
-    <t>2.435*</t>
-  </si>
-  <si>
-    <t>2.697*</t>
-  </si>
-  <si>
     <t>DV: First Law</t>
   </si>
   <si>
@@ -148,6 +100,60 @@
   </si>
   <si>
     <t>0.007*</t>
+  </si>
+  <si>
+    <t>2.093*</t>
+  </si>
+  <si>
+    <t>2.180*</t>
+  </si>
+  <si>
+    <t>3.465*</t>
+  </si>
+  <si>
+    <t>3.611*</t>
+  </si>
+  <si>
+    <t>19.872*</t>
+  </si>
+  <si>
+    <t>6.739*</t>
+  </si>
+  <si>
+    <t>6.517*</t>
+  </si>
+  <si>
+    <t>1.132*</t>
+  </si>
+  <si>
+    <t>5.130*</t>
+  </si>
+  <si>
+    <t>1.138*</t>
+  </si>
+  <si>
+    <t>1.250*</t>
+  </si>
+  <si>
+    <t>1.280*</t>
+  </si>
+  <si>
+    <t>31.369*</t>
+  </si>
+  <si>
+    <t>1.229*</t>
+  </si>
+  <si>
+    <t>1.000</t>
+  </si>
+  <si>
+    <t>0.220</t>
+  </si>
+  <si>
+    <t>0.060</t>
+  </si>
+  <si>
+    <t>1.060</t>
   </si>
 </sst>
 </file>
@@ -651,7 +657,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -675,6 +681,12 @@
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="42">
@@ -997,10 +1009,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A3:G23"/>
+  <dimension ref="A3:G22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -1011,19 +1023,19 @@
   <sheetData>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B3" s="9" t="s">
-        <v>34</v>
+        <v>18</v>
       </c>
       <c r="C3" s="9"/>
       <c r="D3" s="9"/>
       <c r="E3" s="9" t="s">
-        <v>35</v>
+        <v>19</v>
       </c>
       <c r="F3" s="9"/>
       <c r="G3" s="9"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
-        <v>37</v>
+        <v>21</v>
       </c>
       <c r="B4" s="3"/>
       <c r="C4" s="3"/>
@@ -1037,22 +1049,22 @@
         <v>0</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>29</v>
+        <v>15</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>29</v>
+        <v>15</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>29</v>
+        <v>15</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
@@ -1060,22 +1072,22 @@
         <v>1</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>42</v>
+        <v>26</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>42</v>
+        <v>26</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>42</v>
+        <v>26</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>30</v>
+        <v>16</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
@@ -1083,22 +1095,22 @@
         <v>2</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>30</v>
+        <v>16</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>30</v>
+        <v>16</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>30</v>
+        <v>16</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
@@ -1106,22 +1118,22 @@
         <v>3</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>29</v>
+        <v>15</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>29</v>
+        <v>15</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>28</v>
+        <v>14</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>29</v>
+        <v>15</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
@@ -1129,27 +1141,27 @@
         <v>4</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>29</v>
+        <v>15</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>29</v>
+        <v>15</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>28</v>
+        <v>14</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>29</v>
+        <v>15</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>29</v>
+        <v>15</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>29</v>
+        <v>15</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
-        <v>40</v>
+        <v>24</v>
       </c>
       <c r="B10" s="2"/>
       <c r="C10" s="2"/>
@@ -1163,41 +1175,41 @@
         <v>5</v>
       </c>
       <c r="B11" s="8"/>
-      <c r="C11" s="8">
-        <v>1.325</v>
-      </c>
-      <c r="D11" s="8">
-        <v>1.401</v>
+      <c r="C11" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="D11" s="8" t="s">
+        <v>28</v>
       </c>
       <c r="E11" s="8"/>
       <c r="F11" s="8" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="G11" s="8" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="B12" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>26</v>
+      <c r="B12" s="2">
+        <v>0.996</v>
+      </c>
+      <c r="C12" s="2">
+        <v>0.94399999999999995</v>
       </c>
       <c r="D12" s="2">
-        <v>11.584</v>
-      </c>
-      <c r="E12" s="2">
-        <v>14.135999999999999</v>
+        <v>0.30199999999999999</v>
+      </c>
+      <c r="E12" s="11" t="s">
+        <v>42</v>
       </c>
       <c r="F12" s="2">
-        <v>24.440999999999999</v>
-      </c>
-      <c r="G12" s="2">
-        <v>2.6920000000000002</v>
+        <v>0.112</v>
+      </c>
+      <c r="G12" s="11" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
@@ -1205,214 +1217,191 @@
         <v>7</v>
       </c>
       <c r="B13" s="2">
-        <v>1.2290000000000001</v>
-      </c>
-      <c r="C13" s="2">
-        <v>1.121</v>
+        <v>1.0289999999999999</v>
+      </c>
+      <c r="C13" s="11" t="s">
+        <v>44</v>
       </c>
       <c r="D13" s="2">
-        <v>0.34899999999999998</v>
-      </c>
-      <c r="E13" s="2">
-        <v>0.152</v>
-      </c>
-      <c r="F13" s="2">
-        <v>8.5000000000000006E-2</v>
+        <v>0.88300000000000001</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>33</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>8</v>
+        <v>35</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="B14" s="2">
-        <v>1.026</v>
-      </c>
-      <c r="C14" s="2">
-        <v>1.0069999999999999</v>
-      </c>
-      <c r="D14" s="2">
-        <v>0.83899999999999997</v>
-      </c>
-      <c r="E14" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="F14" s="2" t="s">
-        <v>24</v>
-      </c>
+        <v>8</v>
+      </c>
+      <c r="B14" s="2"/>
+      <c r="C14" s="2"/>
+      <c r="D14" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="E14" s="2"/>
+      <c r="F14" s="2"/>
       <c r="G14" s="2" t="s">
-        <v>23</v>
+        <v>31</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="B15" s="2"/>
-      <c r="C15" s="2"/>
-      <c r="D15" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="E15" s="2"/>
-      <c r="F15" s="2"/>
-      <c r="G15" s="2" t="s">
         <v>20</v>
+      </c>
+      <c r="B15" s="2">
+        <v>0.98599999999999999</v>
+      </c>
+      <c r="C15" s="2">
+        <v>0.97899999999999998</v>
+      </c>
+      <c r="D15" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="E15" s="2">
+        <v>0.90900000000000003</v>
+      </c>
+      <c r="F15" s="2">
+        <v>0.92400000000000004</v>
+      </c>
+      <c r="G15" s="2">
+        <v>0.90600000000000003</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F16" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="G16" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="B16" s="2">
-        <v>0.98499999999999999</v>
-      </c>
-      <c r="C16" s="2">
-        <v>0.98199999999999998</v>
-      </c>
-      <c r="D16" s="2">
-        <v>1.002</v>
-      </c>
-      <c r="E16" s="2">
-        <v>0.90600000000000003</v>
-      </c>
-      <c r="F16" s="2">
-        <v>0.91500000000000004</v>
-      </c>
-      <c r="G16" s="2">
-        <v>0.89500000000000002</v>
-      </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="B17" s="2" t="s">
+      <c r="A17" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="C17" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="D17" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="E17" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="F17" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="G17" s="2" t="s">
-        <v>19</v>
-      </c>
+      <c r="B17" s="2"/>
+      <c r="C17" s="2"/>
+      <c r="D17" s="2"/>
+      <c r="E17" s="2"/>
+      <c r="F17" s="2"/>
+      <c r="G17" s="2"/>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="B18" s="2"/>
-      <c r="C18" s="2"/>
-      <c r="D18" s="2"/>
-      <c r="E18" s="2"/>
-      <c r="F18" s="2"/>
-      <c r="G18" s="2"/>
+      <c r="A18" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B18" s="2">
+        <v>152</v>
+      </c>
+      <c r="C18" s="2">
+        <v>152</v>
+      </c>
+      <c r="D18" s="2">
+        <v>152</v>
+      </c>
+      <c r="E18" s="2">
+        <v>152</v>
+      </c>
+      <c r="F18" s="2">
+        <v>152</v>
+      </c>
+      <c r="G18" s="2">
+        <v>152</v>
+      </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="B19" s="2">
-        <v>164</v>
-      </c>
-      <c r="C19" s="2">
-        <v>164</v>
-      </c>
-      <c r="D19" s="2">
-        <v>164</v>
-      </c>
-      <c r="E19" s="2">
-        <v>164</v>
-      </c>
-      <c r="F19" s="2">
-        <v>164</v>
-      </c>
-      <c r="G19" s="2">
-        <v>164</v>
+        <v>10</v>
+      </c>
+      <c r="B19" s="6">
+        <v>7766</v>
+      </c>
+      <c r="C19" s="6">
+        <v>7766</v>
+      </c>
+      <c r="D19" s="6">
+        <v>7766</v>
+      </c>
+      <c r="E19" s="6">
+        <v>12162</v>
+      </c>
+      <c r="F19" s="6">
+        <v>12162</v>
+      </c>
+      <c r="G19" s="6">
+        <v>12162</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="B20" s="6">
-        <v>7870</v>
-      </c>
-      <c r="C20" s="6">
-        <v>7870</v>
-      </c>
-      <c r="D20" s="6">
-        <v>7870</v>
-      </c>
-      <c r="E20" s="6">
-        <v>12269</v>
-      </c>
-      <c r="F20" s="6">
-        <v>12269</v>
-      </c>
-      <c r="G20" s="6">
-        <v>12269</v>
+        <v>11</v>
+      </c>
+      <c r="B20" s="10">
+        <v>-650.47699999999998</v>
+      </c>
+      <c r="C20" s="10">
+        <v>-647.80600000000004</v>
+      </c>
+      <c r="D20" s="10">
+        <v>-643.11400000000003</v>
+      </c>
+      <c r="E20" s="10">
+        <v>-649.44399999999996</v>
+      </c>
+      <c r="F20" s="10">
+        <v>-638.63699999999994</v>
+      </c>
+      <c r="G20" s="10">
+        <v>-635.42899999999997</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="B21" s="2">
-        <v>-657.15</v>
-      </c>
-      <c r="C21" s="2">
-        <v>-656.87</v>
-      </c>
-      <c r="D21" s="2">
-        <v>-651.42200000000003</v>
-      </c>
-      <c r="E21" s="2">
-        <v>-651.74699999999996</v>
-      </c>
-      <c r="F21" s="2">
-        <v>-647.375</v>
-      </c>
-      <c r="G21" s="2">
-        <v>-642.31399999999996</v>
+        <v>25</v>
+      </c>
+      <c r="B21" s="10">
+        <v>1320.9549999999999</v>
+      </c>
+      <c r="C21" s="10">
+        <v>1317.6120000000001</v>
+      </c>
+      <c r="D21" s="10">
+        <v>1310.2270000000001</v>
+      </c>
+      <c r="E21" s="10">
+        <v>1318.8869999999999</v>
+      </c>
+      <c r="F21" s="10">
+        <v>1299.2739999999999</v>
+      </c>
+      <c r="G21" s="10">
+        <v>1294.8579999999999</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A22" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="B22" s="2">
-        <v>1334.299</v>
-      </c>
-      <c r="C22" s="2">
-        <v>1335.739</v>
-      </c>
-      <c r="D22" s="2">
-        <v>1326.8430000000001</v>
-      </c>
-      <c r="E22" s="2">
-        <v>1323.4939999999999</v>
-      </c>
-      <c r="F22" s="2">
-        <v>1316.751</v>
-      </c>
-      <c r="G22" s="2">
-        <v>1308.6279999999999</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A23" s="1" t="s">
-        <v>39</v>
+      <c r="A22" s="1" t="s">
+        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>